<commit_message>
linked admin and verify in react
linked admin and verify in react
</commit_message>
<xml_diff>
--- a/sih-react/public/data/Data.xlsx
+++ b/sih-react/public/data/Data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,21 +443,28 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>CryptoCrux</t>
+          <t>Pandey</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>hello</t>
+          <t>Naina</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>bye</t>
+          <t>Mohit</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Devanshu</t>
         </is>
       </c>
     </row>

</xml_diff>